<commit_message>
Adding Module 04 Content
</commit_message>
<xml_diff>
--- a/17. LinkedIn Learning/01. Microsoft Excel/01. Master Microsoft Excel - Learning Path/04. Excel - Creating a basic dashboard/Material/Ex_Files_Dashboard_Excel2016/Exercise Files/Chapter01/Conditional.xlsx
+++ b/17. LinkedIn Learning/01. Microsoft Excel/01. Master Microsoft Excel - Learning Path/04. Excel - Creating a basic dashboard/Material/Ex_Files_Dashboard_Excel2016/Exercise Files/Chapter01/Conditional.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Curt\Desktop\Exercise Files\Chapter01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Descargas\1. GIT\OnlineCourses\17. LinkedIn Learning\01. Microsoft Excel\01. Master Microsoft Excel - Learning Path\04. Excel - Creating a basic dashboard\Material\Ex_Files_Dashboard_Excel2016\Exercise Files\Chapter01\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F3660A-9729-47A2-87A1-E3E1560072BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27195" windowHeight="14820"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -47,10 +48,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -123,25 +124,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Currency" xfId="3" builtinId="4"/>
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Moneda" xfId="3" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -155,7 +177,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -474,29 +496,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C1" s="6">
-        <v>1200000</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1250000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
@@ -504,13 +526,13 @@
         <v>2400000</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2014</v>
       </c>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>0</v>
       </c>
@@ -518,15 +540,15 @@
         <v>1111886</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="1">
         <v>1214733</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
@@ -534,13 +556,13 @@
         <v>2326619</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>2015</v>
       </c>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>0</v>
       </c>
@@ -548,15 +570,15 @@
         <v>1286966</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="1">
         <v>1523054</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>3</v>
       </c>
@@ -565,6 +587,21 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C5">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>C5&gt;=$C$1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>C6&gt;=$C$1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9:C10">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>C9&gt;=$C$1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>